<commit_message>
understanding pickle file structure
</commit_message>
<xml_diff>
--- a/test_output/output.xlsx
+++ b/test_output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,22 +434,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>data</t>
-        </is>
+      <c r="A1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>14</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t xml:space="preserve">                      Time Driver                LapTime  NumberOfLaps  NumberOfPitStops  ... SpeedI1 SpeedI2 SpeedFL SpeedST IsPersonalBest
 0   0 days 01:03:58.671000      1                    NaT             1                 0  ...   274.0   293.0   273.0   239.0          False
@@ -466,12 +462,7 @@
 [995 rows x 18 columns]</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>14</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t xml:space="preserve">                        Time Driver  Position GapToLeader IntervalToPositionAhead
 0     0 days 00:00:06.078000      1         1       LAP 1                   LAP 1
@@ -488,12 +479,7 @@
 [21024 rows x 5 columns]</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>14</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>[datetime.timedelta(0), datetime.timedelta(days=1), datetime.timedelta(days=1)]</t>
         </is>

</xml_diff>